<commit_message>
edited some table columns
</commit_message>
<xml_diff>
--- a/BackEnd/alltables.xlsx
+++ b/BackEnd/alltables.xlsx
@@ -53,9 +53,6 @@
     <t>genre_id  integer</t>
   </si>
   <si>
-    <t>genre      charvar(20)</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>gender    char(1)</t>
   </si>
   <si>
-    <t>age_range integer</t>
-  </si>
-  <si>
     <t>occupation  charvar(30)</t>
   </si>
   <si>
@@ -110,12 +104,6 @@
     <t>DOB               charvar(20)</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>role_id   integer</t>
-  </si>
-  <si>
     <t>Name         text</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t xml:space="preserve">date            date </t>
   </si>
   <si>
-    <t>rating       integer</t>
-  </si>
-  <si>
     <t>MovieGenre</t>
   </si>
   <si>
@@ -243,6 +228,21 @@
   </si>
   <si>
     <t>UserCreates  Profile</t>
+  </si>
+  <si>
+    <t>age integer</t>
+  </si>
+  <si>
+    <t>Time_stamp time</t>
+  </si>
+  <si>
+    <t>name     charvar(20)</t>
+  </si>
+  <si>
+    <t>Plays in</t>
+  </si>
+  <si>
+    <t>duration     time</t>
   </si>
 </sst>
 </file>
@@ -633,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,26 +650,30 @@
     <col min="8" max="8" width="10.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="12" width="10.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="1" customWidth="1"/>
     <col min="13" max="15" width="8.88671875" style="1"/>
     <col min="16" max="16" width="10.21875" style="1" customWidth="1"/>
-    <col min="17" max="18" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="11" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="1"/>
     <col min="19" max="19" width="10.77734375" style="1" customWidth="1"/>
     <col min="20" max="20" width="10.6640625" style="1" customWidth="1"/>
     <col min="21" max="21" width="10.5546875" style="1" customWidth="1"/>
     <col min="22" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -688,39 +692,57 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -728,15 +750,21 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="1:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -744,68 +772,69 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-    </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="7" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="D9" s="3"/>
@@ -813,13 +842,11 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="D10" s="3"/>
@@ -827,56 +854,54 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="K13" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -888,7 +913,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -900,44 +925,44 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -947,7 +972,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -957,41 +982,44 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="E24" s="3"/>
@@ -999,8 +1027,9 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="E25" s="3"/>
@@ -1008,42 +1037,43 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-    </row>
-    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1052,7 +1082,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1061,54 +1091,26 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="32" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new EER diagram. modified alltables.xlsx
</commit_message>
<xml_diff>
--- a/BackEnd/alltables.xlsx
+++ b/BackEnd/alltables.xlsx
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,10 +666,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -798,7 +798,7 @@
       <c r="G7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -824,13 +824,13 @@
       <c r="I8" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="K8" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="L8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -842,9 +842,9 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
@@ -854,9 +854,9 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">

</xml_diff>

<commit_message>
added all queries to set up database
</commit_message>
<xml_diff>
--- a/BackEnd/alltables.xlsx
+++ b/BackEnd/alltables.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11364" windowHeight="5088"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11364" windowHeight="5088" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="227">
   <si>
     <t>Movies</t>
   </si>
@@ -369,6 +370,342 @@
   </si>
   <si>
     <t>Tom Tykwer</t>
+  </si>
+  <si>
+    <t>The Shawshank Redemption</t>
+  </si>
+  <si>
+    <t>The Godfather: Part II</t>
+  </si>
+  <si>
+    <t>Schindler's List</t>
+  </si>
+  <si>
+    <t>Pulp Fiction</t>
+  </si>
+  <si>
+    <t>12 Angry Men</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: The Return of the King</t>
+  </si>
+  <si>
+    <t>The Good, the Bad and the Ugly</t>
+  </si>
+  <si>
+    <t>Fight Club</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: The Fellowship of the Ring</t>
+  </si>
+  <si>
+    <t>Star Wars: Episode V - The Empire Strikes Back</t>
+  </si>
+  <si>
+    <t>Forrest Gump</t>
+  </si>
+  <si>
+    <t>Inception</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: The Two Towers</t>
+  </si>
+  <si>
+    <t>One Flew Over the Cuckoo's Nest</t>
+  </si>
+  <si>
+    <t>Goodfellas</t>
+  </si>
+  <si>
+    <t>The Matrix</t>
+  </si>
+  <si>
+    <t>Seven Samurai</t>
+  </si>
+  <si>
+    <t>Star Wars: Episode IV - A New Hope</t>
+  </si>
+  <si>
+    <t>City of God</t>
+  </si>
+  <si>
+    <t>Se7en</t>
+  </si>
+  <si>
+    <t>The Silence of the Lambs</t>
+  </si>
+  <si>
+    <t>It's a Wonderful Life</t>
+  </si>
+  <si>
+    <t>The Usual Suspects</t>
+  </si>
+  <si>
+    <t>Life Is Beautiful</t>
+  </si>
+  <si>
+    <t>LÃ©on: The Professional</t>
+  </si>
+  <si>
+    <t>Once Upon a Time in the West</t>
+  </si>
+  <si>
+    <t>Spirited Away</t>
+  </si>
+  <si>
+    <t>Saving Private Ryan</t>
+  </si>
+  <si>
+    <t>Interstellar</t>
+  </si>
+  <si>
+    <t>Casablanca</t>
+  </si>
+  <si>
+    <t>American History X</t>
+  </si>
+  <si>
+    <t>City Lights</t>
+  </si>
+  <si>
+    <t>Psycho</t>
+  </si>
+  <si>
+    <t>Raiders of the Lost Ark</t>
+  </si>
+  <si>
+    <t>Rear Window</t>
+  </si>
+  <si>
+    <t>The Intouchables</t>
+  </si>
+  <si>
+    <t>Modern Times</t>
+  </si>
+  <si>
+    <t>The Green Mile</t>
+  </si>
+  <si>
+    <t>Frank Darabont</t>
+  </si>
+  <si>
+    <t>Steven Spielberg</t>
+  </si>
+  <si>
+    <t>Quentin Tarantino</t>
+  </si>
+  <si>
+    <t>Sidney Lumet</t>
+  </si>
+  <si>
+    <t>Peter Jackson</t>
+  </si>
+  <si>
+    <t>Sergio Leone</t>
+  </si>
+  <si>
+    <t>David Fincher</t>
+  </si>
+  <si>
+    <t>Irvin Kershner</t>
+  </si>
+  <si>
+    <t>Robert Zemeckis</t>
+  </si>
+  <si>
+    <t>Milos Forman</t>
+  </si>
+  <si>
+    <t>Martin Scorsese</t>
+  </si>
+  <si>
+    <t>Lana Wachowski, Lilly Wachowski</t>
+  </si>
+  <si>
+    <t>Akira Kurosawa</t>
+  </si>
+  <si>
+    <t>George Lucas</t>
+  </si>
+  <si>
+    <t>Fernando Meirelles, KÃ¡tia Lund</t>
+  </si>
+  <si>
+    <t>Jonathan Demme</t>
+  </si>
+  <si>
+    <t>Frank Capra</t>
+  </si>
+  <si>
+    <t>Bryan Singer</t>
+  </si>
+  <si>
+    <t>Roberto Benigni</t>
+  </si>
+  <si>
+    <t>Luc Besson</t>
+  </si>
+  <si>
+    <t>Hayao Miyazaki</t>
+  </si>
+  <si>
+    <t>Michael Curtiz</t>
+  </si>
+  <si>
+    <t>Tony Kaye</t>
+  </si>
+  <si>
+    <t>Charles Chaplin</t>
+  </si>
+  <si>
+    <t>Alfred Hitchcock</t>
+  </si>
+  <si>
+    <t>Olivier Nakache, Eric Toledano</t>
+  </si>
+  <si>
+    <t>Charles Chaplin (as Charlie Chaplin)</t>
+  </si>
+  <si>
+    <t>15, 16</t>
+  </si>
+  <si>
+    <t>6, 7</t>
+  </si>
+  <si>
+    <t>21, 22</t>
+  </si>
+  <si>
+    <t>Marlon Brando, Al Pacino, James Caan</t>
+  </si>
+  <si>
+    <t>Al Pacino, Robert De Niro, Robert Duvall</t>
+  </si>
+  <si>
+    <t>Christian Bale, Heath Ledger, Aaron Eckhart</t>
+  </si>
+  <si>
+    <t>Liam Neeson, Ralph Fiennes, Ben Kingsley</t>
+  </si>
+  <si>
+    <t>John Travolta, Uma Thurman, Samuel L. Jackson</t>
+  </si>
+  <si>
+    <t>Henry Fonda, Lee J. Cobb, Martin Balsam</t>
+  </si>
+  <si>
+    <t>Elijah Wood, Viggo Mortensen, Ian McKellen</t>
+  </si>
+  <si>
+    <t>Clint Eastwood, Eli Wallach, Lee Van Cleef</t>
+  </si>
+  <si>
+    <t>Brad Pitt, Edward Norton, Helena Bonham Carter</t>
+  </si>
+  <si>
+    <t>Elijah Wood, Ian McKellen, Orlando Bloom</t>
+  </si>
+  <si>
+    <t>Mark Hamill, Harrison Ford, Carrie Fisher</t>
+  </si>
+  <si>
+    <t>Tom Hanks, Robin Wright, Gary Sinise</t>
+  </si>
+  <si>
+    <t>Leonardo DiCaprio, Joseph Gordon-Levitt, Ellen Page</t>
+  </si>
+  <si>
+    <t>Elijah Wood, Ian McKellen, Viggo Mortensen</t>
+  </si>
+  <si>
+    <t>Jack Nicholson, Louise Fletcher, Michael Berryman</t>
+  </si>
+  <si>
+    <t>Robert De Niro, Ray Liotta, Joe Pesci</t>
+  </si>
+  <si>
+    <t>Keanu Reeves, Laurence Fishburne, Carrie-Anne Moss</t>
+  </si>
+  <si>
+    <t>ToshirÃ´ Mifune, Takashi Shimura, Keiko Tsushima</t>
+  </si>
+  <si>
+    <t>Alexandre Rodrigues, Matheus Nachtergaele, Leandro Firmino</t>
+  </si>
+  <si>
+    <t>Morgan Freeman, Brad Pitt, Kevin Spacey</t>
+  </si>
+  <si>
+    <t>Jodie Foster, Anthony Hopkins, Lawrence A. Bonney</t>
+  </si>
+  <si>
+    <t>James Stewart, Donna Reed, Lionel Barrymore</t>
+  </si>
+  <si>
+    <t>Kevin Spacey, Gabriel Byrne, Chazz Palminteri</t>
+  </si>
+  <si>
+    <t>Roberto Benigni, Nicoletta Braschi, Giorgio Cantarini</t>
+  </si>
+  <si>
+    <t>Jean Reno, Gary Oldman, Natalie Portman</t>
+  </si>
+  <si>
+    <t>Henry Fonda, Charles Bronson, Claudia Cardinale</t>
+  </si>
+  <si>
+    <t>Daveigh Chase, Suzanne Pleshette, Miyu Irino</t>
+  </si>
+  <si>
+    <t>Tom Hanks, Matt Damon, Tom Sizemore</t>
+  </si>
+  <si>
+    <t>Matthew McConaughey, Anne Hathaway, Jessica Chastain</t>
+  </si>
+  <si>
+    <t>Humphrey Bogart, Ingrid Bergman, Paul Henreid</t>
+  </si>
+  <si>
+    <t>Edward Norton, Edward Furlong, Beverly D'Angelo</t>
+  </si>
+  <si>
+    <t>Charles Chaplin, Virginia Cherrill, Florence Lee</t>
+  </si>
+  <si>
+    <t>Anthony Perkins, Janet Leigh, Vera Miles</t>
+  </si>
+  <si>
+    <t>Harrison Ford, Karen Allen, Paul Freeman</t>
+  </si>
+  <si>
+    <t>James Stewart, Grace Kelly, Wendell Corey</t>
+  </si>
+  <si>
+    <t>FranÃ§ois Cluzet, Omar Sy, Anne Le Ny</t>
+  </si>
+  <si>
+    <t>Charles Chaplin, Paulette Goddard, Henry Bergman</t>
+  </si>
+  <si>
+    <t>Tom Hanks, Michael Clarke Duncan, David Morse</t>
+  </si>
+  <si>
+    <t>92, 75, 10</t>
+  </si>
+  <si>
+    <t>67, 2, 44</t>
+  </si>
+  <si>
+    <t>2, 85, 86</t>
+  </si>
+  <si>
+    <t>17, 36, 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63, 83, </t>
+  </si>
+  <si>
+    <t>Tim RobbB1:E32ins, Morgan Freeman, Bob Gunton</t>
   </si>
 </sst>
 </file>
@@ -519,7 +856,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,6 +1040,24 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -882,7 +1237,7 @@
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -907,6 +1262,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1265,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,4 +2352,601 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="70.44140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="48.5546875" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="G24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="G26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="G32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="G38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>